<commit_message>
actualizacion Vo.Bo. UPP 4T 2020 SIPOT
</commit_message>
<xml_diff>
--- a/xlsx/a69_f01UPPachuca.xlsx
+++ b/xlsx/a69_f01UPPachuca.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2DA ENTREGA DEL REPORTE DE LAS 48 FRACCIONES COMUNES\ENTREGA 3ER TRIMESTRE DE LAS 48 FRACIONES COMUNES\Vo. Bo. #1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\MAYDELI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="5895"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
@@ -338,7 +338,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="justify" wrapText="1"/>
     </xf>
@@ -362,6 +361,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -643,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,46 +665,46 @@
     <col min="12" max="12" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="9" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -742,7 +742,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -780,23 +780,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:17" ht="39" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" ht="39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -834,128 +834,113 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>2020</v>
       </c>
-      <c r="B8" s="8">
-        <v>44013</v>
-      </c>
-      <c r="C8" s="8">
-        <v>44104</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="B8" s="7">
+        <v>44105</v>
+      </c>
+      <c r="C8" s="7">
+        <v>44196</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>38061</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>39469</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="5">
-        <v>44114</v>
-      </c>
-      <c r="K8" s="5">
-        <v>44114</v>
-      </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="J8" s="4">
+        <v>44206</v>
+      </c>
+      <c r="K8" s="4">
+        <v>44206</v>
+      </c>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>2020</v>
       </c>
-      <c r="B9" s="8">
-        <v>44013</v>
-      </c>
-      <c r="C9" s="8">
-        <v>44104</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="B9" s="7">
+        <v>44105</v>
+      </c>
+      <c r="C9" s="7">
+        <v>44196</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>39622</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>39622</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="5">
-        <v>44114</v>
-      </c>
-      <c r="K9" s="5">
-        <v>44114</v>
-      </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:17" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="J9" s="4">
+        <v>44206</v>
+      </c>
+      <c r="K9" s="4">
+        <v>44206</v>
+      </c>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>2020</v>
       </c>
-      <c r="B10" s="8">
-        <v>44013</v>
-      </c>
-      <c r="C10" s="8">
-        <v>44104</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="B10" s="7">
+        <v>44105</v>
+      </c>
+      <c r="C10" s="7">
+        <v>44196</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>43465</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>43465</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="5">
-        <v>44114</v>
-      </c>
-      <c r="K10" s="5">
-        <v>44114</v>
-      </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
+      <c r="J10" s="4">
+        <v>44206</v>
+      </c>
+      <c r="K10" s="4">
+        <v>44206</v>
+      </c>
+      <c r="L10" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -986,157 +971,162 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="11" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="11" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="11" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="11" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="11" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="11" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="11" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="11" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualizacion de febrero hay un archivo mal
</commit_message>
<xml_diff>
--- a/xlsx/a69_f01UPPachuca.xlsx
+++ b/xlsx/a69_f01UPPachuca.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\SIPOT 3ER TRIMETRES 2021\Recepción de Información\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2022\SIPOT\4to trimestre 2021\4to Trimestre SIPOT 2021 Pagina Oficial\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,7 +673,7 @@
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" customWidth="1"/>
     <col min="6" max="6" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="102" customWidth="1"/>
@@ -857,10 +857,10 @@
         <v>2021</v>
       </c>
       <c r="B8" s="9">
-        <v>44378</v>
+        <v>44470</v>
       </c>
       <c r="C8" s="9">
-        <v>44469</v>
+        <v>44561</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>50</v>
@@ -881,10 +881,10 @@
         <v>69</v>
       </c>
       <c r="J8" s="8">
-        <v>44480</v>
+        <v>44571</v>
       </c>
       <c r="K8" s="9">
-        <v>44480</v>
+        <v>44571</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="2"/>
@@ -898,10 +898,10 @@
         <v>2021</v>
       </c>
       <c r="B9" s="9">
-        <v>44378</v>
+        <v>44470</v>
       </c>
       <c r="C9" s="9">
-        <v>44469</v>
+        <v>44561</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>42</v>
@@ -922,10 +922,10 @@
         <v>69</v>
       </c>
       <c r="J9" s="9">
-        <v>44480</v>
+        <v>44571</v>
       </c>
       <c r="K9" s="9">
-        <v>44480</v>
+        <v>44571</v>
       </c>
       <c r="L9" s="4"/>
     </row>
@@ -934,10 +934,10 @@
         <v>2021</v>
       </c>
       <c r="B10" s="9">
-        <v>44378</v>
+        <v>44470</v>
       </c>
       <c r="C10" s="9">
-        <v>44469</v>
+        <v>44561</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>68</v>
@@ -958,10 +958,10 @@
         <v>69</v>
       </c>
       <c r="J10" s="9">
-        <v>44480</v>
+        <v>44571</v>
       </c>
       <c r="K10" s="9">
-        <v>44480</v>
+        <v>44571</v>
       </c>
       <c r="L10" s="4"/>
     </row>

</xml_diff>

<commit_message>
cambios de may de mayo
</commit_message>
<xml_diff>
--- a/xlsx/a69_f01UPPachuca.xlsx
+++ b/xlsx/a69_f01UPPachuca.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2022\SIPOT\4to trimestre 2021\4to Trimestre SIPOT 2021 Pagina Oficial\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2022\SIPOT\1er Trimestre 2022\Recepción de Información\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
@@ -232,34 +232,31 @@
     <t>Otro</t>
   </si>
   <si>
+    <t>Decreto que Modifica Diversas Disposiciones del Diverso que Abrogó al que Creó a la Universidad Politécnica de Pachuca, Publicado en el Periódico oficial del estado el 15 de marzo de 2004.</t>
+  </si>
+  <si>
+    <t>http://www.upp.edu.mx/normatividad/files/interna/decretos/decreto-de-creacion-vigente-04_02_2008.pdf</t>
+  </si>
+  <si>
     <t>Abogado General (UPP)</t>
   </si>
   <si>
-    <t>Decreto que Modifica Diversas Disposiciones del Diverso que Abrogó al que Creó a la Universidad Politécnica de Pachuca, Publicado en el Periódico oficial del estado el 15 de marzo de 2004.</t>
-  </si>
-  <si>
     <t>Estatuto Orgánico de la Universidad Politécnica de Pachuca</t>
   </si>
   <si>
     <t>http://www.upp.edu.mx/normatividad/files/interna/estatutos/estatuto-organico-de-la-universidad-politecnica-de-pachuca-25_08_2008.pdf</t>
   </si>
   <si>
-    <t>http://www.upp.edu.mx/normatividad/files/interna/decretos/decreto-de-creacion-vigente-04_02_2008.pdf</t>
+    <t>Cuotas y Tarifas del Organismo Descentralizado de la Administración Pública Estatal denominado Universidad Politécnica de Pachuca 2021</t>
   </si>
   <si>
     <t>https://periodico.hidalgo.gob.mx/?tribe_events=periodico-oficial-alcance-3-del-31-de-diciembre-de-2020</t>
-  </si>
-  <si>
-    <t>Cuotas y Tarifas del Organismo Descentralizado de la Administración Pública Estatal denominado Universidad Politécnica de Pachuca 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -273,25 +270,22 @@
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -339,50 +333,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="justify" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Millares 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -663,8 +652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,14 +662,14 @@
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" customWidth="1"/>
     <col min="6" max="6" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="102" customWidth="1"/>
-    <col min="9" max="9" width="40.42578125" customWidth="1"/>
+    <col min="8" max="8" width="83.85546875" customWidth="1"/>
+    <col min="9" max="9" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -689,38 +678,38 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -799,22 +788,22 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:17" ht="39" x14ac:dyDescent="0.25">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -852,122 +841,128 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
-        <v>2021</v>
-      </c>
-      <c r="B8" s="9">
-        <v>44470</v>
-      </c>
-      <c r="C8" s="9">
-        <v>44561</v>
-      </c>
-      <c r="D8" s="4" t="s">
+    <row r="8" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B8" s="4">
+        <v>44562</v>
+      </c>
+      <c r="C8" s="4">
+        <v>44651</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="8">
+        <v>39482</v>
+      </c>
+      <c r="G8" s="8">
+        <v>39469</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F8" s="5">
-        <v>39482</v>
-      </c>
-      <c r="G8" s="6">
-        <v>39469</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="4">
+        <v>44659</v>
+      </c>
+      <c r="K8" s="4">
+        <v>44659</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B9" s="4">
+        <v>44562</v>
+      </c>
+      <c r="C9" s="4">
+        <v>44651</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="8">
+        <v>39685</v>
+      </c>
+      <c r="G9" s="8">
+        <v>39622</v>
+      </c>
+      <c r="H9" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="8">
-        <v>44571</v>
-      </c>
-      <c r="K8" s="9">
-        <v>44571</v>
-      </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-    </row>
-    <row r="9" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>2021</v>
-      </c>
-      <c r="B9" s="9">
-        <v>44470</v>
-      </c>
-      <c r="C9" s="9">
-        <v>44561</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="I9" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F9" s="5">
-        <v>39685</v>
-      </c>
-      <c r="G9" s="6">
-        <v>39622</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="9">
-        <v>44571</v>
-      </c>
-      <c r="K9" s="9">
-        <v>44571</v>
-      </c>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
-        <v>2021</v>
-      </c>
-      <c r="B10" s="9">
-        <v>44470</v>
-      </c>
-      <c r="C10" s="9">
-        <v>44561</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="J9" s="4">
+        <v>44659</v>
+      </c>
+      <c r="K9" s="4">
+        <v>44659</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+    </row>
+    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B10" s="4">
+        <v>44562</v>
+      </c>
+      <c r="C10" s="4">
+        <v>44651</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="8">
+        <v>44196</v>
+      </c>
+      <c r="G10" s="8">
+        <v>44196</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="5">
-        <v>44196</v>
-      </c>
-      <c r="G10" s="5">
-        <v>44196</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10" s="9">
-        <v>44571</v>
-      </c>
-      <c r="K10" s="9">
-        <v>44571</v>
-      </c>
-      <c r="L10" s="4"/>
+      <c r="I10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" s="4">
+        <v>44659</v>
+      </c>
+      <c r="K10" s="4">
+        <v>44659</v>
+      </c>
+      <c r="L10" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A6:L6"/>
+    <mergeCell ref="M9:Q9"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
@@ -976,7 +971,7 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D8:D10">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D11:D200">
       <formula1>Hidden_13</formula1>
     </dataValidation>
   </dataValidations>
@@ -986,7 +981,7 @@
     <hyperlink ref="H10" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
cambios de agosto, puntos fe de ratas e historico
</commit_message>
<xml_diff>
--- a/xlsx/a69_f01UPPachuca.xlsx
+++ b/xlsx/a69_f01UPPachuca.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2022\SIPOT\1er Trimestre 2022\Recepción de Información\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8355"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
@@ -235,22 +230,22 @@
     <t>Decreto que Modifica Diversas Disposiciones del Diverso que Abrogó al que Creó a la Universidad Politécnica de Pachuca, Publicado en el Periódico oficial del estado el 15 de marzo de 2004.</t>
   </si>
   <si>
-    <t>http://www.upp.edu.mx/normatividad/files/interna/decretos/decreto-de-creacion-vigente-04_02_2008.pdf</t>
-  </si>
-  <si>
     <t>Abogado General (UPP)</t>
   </si>
   <si>
     <t>Estatuto Orgánico de la Universidad Politécnica de Pachuca</t>
   </si>
   <si>
-    <t>http://www.upp.edu.mx/normatividad/files/interna/estatutos/estatuto-organico-de-la-universidad-politecnica-de-pachuca-25_08_2008.pdf</t>
-  </si>
-  <si>
     <t>Cuotas y Tarifas del Organismo Descentralizado de la Administración Pública Estatal denominado Universidad Politécnica de Pachuca 2021</t>
   </si>
   <si>
-    <t>https://periodico.hidalgo.gob.mx/?tribe_events=periodico-oficial-alcance-3-del-31-de-diciembre-de-2020</t>
+    <t>https://periodico.hidalgo.gob.mx/?tribe_events=periodico-oficial-alcance-9-del-31-de-diciembre-de-2021</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/interna/estatutos/estatuto-organico-de-la-universidad-politecnica-de-pachuca-25_08_2008.pdf</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/interna/decretos/decreto-de-creacion-vigente-04_02_2008.pdf</t>
   </si>
 </sst>
 </file>
@@ -270,11 +265,13 @@
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -642,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -652,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,10 +843,10 @@
         <v>2022</v>
       </c>
       <c r="B8" s="4">
-        <v>44562</v>
+        <v>44652</v>
       </c>
       <c r="C8" s="4">
-        <v>44651</v>
+        <v>44742</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>50</v>
@@ -864,16 +861,16 @@
         <v>39469</v>
       </c>
       <c r="H8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>71</v>
-      </c>
       <c r="J8" s="4">
-        <v>44659</v>
+        <v>44753</v>
       </c>
       <c r="K8" s="4">
-        <v>44659</v>
+        <v>44753</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="5"/>
@@ -887,16 +884,16 @@
         <v>2022</v>
       </c>
       <c r="B9" s="4">
-        <v>44562</v>
+        <v>44652</v>
       </c>
       <c r="C9" s="4">
-        <v>44651</v>
+        <v>44742</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="8">
         <v>39685</v>
@@ -905,16 +902,16 @@
         <v>39622</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" s="4">
-        <v>44659</v>
+        <v>44753</v>
       </c>
       <c r="K9" s="4">
-        <v>44659</v>
+        <v>44753</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="12"/>
@@ -928,34 +925,34 @@
         <v>2022</v>
       </c>
       <c r="B10" s="4">
-        <v>44562</v>
+        <v>44652</v>
       </c>
       <c r="C10" s="4">
-        <v>44651</v>
+        <v>44742</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F10" s="8">
-        <v>44196</v>
+        <v>44539</v>
       </c>
       <c r="G10" s="8">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J10" s="4">
-        <v>44659</v>
+        <v>44753</v>
       </c>
       <c r="K10" s="4">
-        <v>44659</v>
+        <v>44753</v>
       </c>
       <c r="L10" s="2"/>
     </row>
@@ -971,17 +968,12 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D11:D200">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D11:D107">
       <formula1>Hidden_13</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1"/>
-    <hyperlink ref="H9" r:id="rId2"/>
-    <hyperlink ref="H10" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
cambio de fracciones e historico
</commit_message>
<xml_diff>
--- a/xlsx/a69_f01UPPachuca.xlsx
+++ b/xlsx/a69_f01UPPachuca.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="8355"/>
+    <workbookView xWindow="750" yWindow="555" windowWidth="13815" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="Hidden_13">Hidden_1!$A$1:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="113">
   <si>
     <t>43958</t>
   </si>
@@ -227,32 +227,143 @@
     <t>Otro</t>
   </si>
   <si>
+    <t>Abogado General (UPP)</t>
+  </si>
+  <si>
     <t>Decreto que Modifica Diversas Disposiciones del Diverso que Abrogó al que Creó a la Universidad Politécnica de Pachuca, Publicado en el Periódico oficial del estado el 15 de marzo de 2004.</t>
   </si>
   <si>
-    <t>Abogado General (UPP)</t>
+    <t>https://www.upp.edu.mx/normatividad/files/interna/decretos/decreto-de-creacion-vigente-04_02_2008.pdf</t>
   </si>
   <si>
     <t>Estatuto Orgánico de la Universidad Politécnica de Pachuca</t>
   </si>
   <si>
-    <t>Cuotas y Tarifas del Organismo Descentralizado de la Administración Pública Estatal denominado Universidad Politécnica de Pachuca 2021</t>
+    <t>https://www.upp.edu.mx/normatividad/files/interna/estatutos/estatuto-organico-de-la-universidad-politecnica-de-pachuca-25_08_2008.pdf</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/federal/Constitucion-Pol%C3%ADtica-de-los-Estados-Unidos-Mexicanos.pdf</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/federal/ley-de-adquisiciones-arrendamientos-y-servicios-del-sector-publico.pdf</t>
+  </si>
+  <si>
+    <t>Ley de Adqusiciones, Arrendamientos y Servicios del Sector Público</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/federal/ley-de-disciplina-financiera-de-las-entidades-federales-y-los-municipios.pdf</t>
+  </si>
+  <si>
+    <t>Ley de Disciplina Financiera de las Entidades Federales y los Municipios</t>
+  </si>
+  <si>
+    <t>Ley Federal de Transparencia y Acceso a la Información Pública</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/federal/ley-federal-de-transparencia-y-acceso-a-la-informacion-publica.pdf</t>
+  </si>
+  <si>
+    <t>Ley General de Archivos</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/federal/ley-general-de-archivos.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constitución Política del Estado de Hidalgo </t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/estatal/constitucion-politica-del-estado-de-hidalgo-16-10-17.pdf</t>
+  </si>
+  <si>
+    <t>Ley de Adquisiciones, Arrendamientos y Servicios del Sector Público del Estado de Hidalgo</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/estatal/ley-de-adquisiciones-arrendamientos-y-servicios-del-sector-publico-del-estado-de-hidalgo.pdf</t>
+  </si>
+  <si>
+    <t>Ley de Educación para el Estado de Hidalgo</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/estatal/ley-de-educacion-para-el-estado-de-hidalgo.pdf</t>
+  </si>
+  <si>
+    <t>Ley de los Trabajadores al Servicio de los Gobiernos Estatal y Municipales, así como de los Organismos Descentralizados del Estado de Hidalgo</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/estatal/ley-de-los-trabajadores-al-servicio-de-los-gobiernos-estatal-y-municipales.pdf</t>
+  </si>
+  <si>
+    <t>Ley de Transparencia y Acceso a la Información Pública para el Estado de Hidalgo</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/estatal/ley-de-transparencia-y-acceso-a-la-informacion-publica-para-el-estado-de-hidalgo.pdf</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/estatal/ley-de-archivos-del-estado-de-hidalgo-07_05_2007.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reglamento de la Ley de Adquisiciones arrendamientos y servicios del Sector Público del Estado de Hidalgo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ley de Archivos del Estado de Hidalgo </t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/estatal/reglamento-de-la-ley-de-adquisiciones-arrendamientos-y-servicios-del-sector-publico-del-estado-de-hidalgo-30_09_2004.pdf</t>
+  </si>
+  <si>
+    <t>Reglamento Ley de Entidades Paraestatales de Hidalgo</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/externa/estatal/Reglamento_Ley_de_entidades_Paraestatales_de_Hidalgo_06_08_2021.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comité de Control y Desempeno Institucional </t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/interna/cocodi/comite-de-control-y-desempenno-institucional-cocodi.pdf</t>
+  </si>
+  <si>
+    <t>Código de Ética de la Administración Publica del Estado de Hidalgo</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/interna/codigos/Codigo-de-Etica-de-la-Administracion-Publica-del-Estado-de-Hidalgo.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normas para la desincorporación de bienes de la UPPachuca </t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/interna/normas/normas-para-la-desincorporacion-de-bienes-de-la-uppachuca-19_09_11.pdf</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/interna/manuales/manual-de-organizacion-2020.pdf</t>
+  </si>
+  <si>
+    <t>Manual de Organización</t>
+  </si>
+  <si>
+    <t>https://www.upp.edu.mx/normatividad/files/interna/manuales/MP_UPP_validado_SEPTIEMBRE_2021.pdf</t>
+  </si>
+  <si>
+    <t>Manual de Procedimientos</t>
+  </si>
+  <si>
+    <t>Ley de Entidades Paraestatales</t>
+  </si>
+  <si>
+    <t>http://www.congreso-hidalgo.gob.mx/biblioteca_legislativa/leyes_cintillo/Ley%20de%20Entidades%20Paraestatales%20del%20Estado%20de%20Hidalgo.pdf</t>
+  </si>
+  <si>
+    <t>Cuotas y Tarifas 2022</t>
   </si>
   <si>
     <t>https://periodico.hidalgo.gob.mx/?tribe_events=periodico-oficial-alcance-9-del-31-de-diciembre-de-2021</t>
-  </si>
-  <si>
-    <t>https://www.upp.edu.mx/normatividad/files/interna/estatutos/estatuto-organico-de-la-universidad-politecnica-de-pachuca-25_08_2008.pdf</t>
-  </si>
-  <si>
-    <t>https://www.upp.edu.mx/normatividad/files/interna/decretos/decreto-de-creacion-vigente-04_02_2008.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -265,13 +376,11 @@
       <sz val="11"/>
       <color indexed="9"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -283,6 +392,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF3333CC"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -334,24 +457,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -359,13 +478,43 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -373,12 +522,17 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3333CC"/>
+      <color rgb="FF0066FF"/>
+      <color rgb="FF6600FF"/>
+      <color rgb="FF6666FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -395,39 +549,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -462,7 +616,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -506,151 +660,175 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,56 +837,56 @@
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" customWidth="1"/>
     <col min="6" max="6" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="83.85546875" customWidth="1"/>
+    <col min="8" max="8" width="88.42578125" customWidth="1"/>
     <col min="9" max="9" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="10" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="14" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="14" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -746,7 +924,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -784,23 +962,23 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-    </row>
-    <row r="7" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+    </row>
+    <row r="7" spans="1:12" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -838,128 +1016,801 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>2022</v>
-      </c>
-      <c r="B8" s="4">
-        <v>44652</v>
-      </c>
-      <c r="C8" s="4">
-        <v>44742</v>
-      </c>
-      <c r="D8" s="6" t="s">
+    <row r="8" spans="1:12" s="4" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B8" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C8" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="12">
+        <v>6246</v>
+      </c>
+      <c r="G8" s="12">
+        <v>44344</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K8" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B9" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C9" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="12">
+        <v>36529</v>
+      </c>
+      <c r="G9" s="12">
+        <v>44336</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K9" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B10" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C10" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="12">
+        <v>42487</v>
+      </c>
+      <c r="G10" s="12">
+        <v>43130</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K10" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B11" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C11" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="12">
+        <v>42499</v>
+      </c>
+      <c r="G11" s="12">
+        <v>44336</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K11" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B12" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C12" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="12">
+        <v>43266</v>
+      </c>
+      <c r="G12" s="12">
+        <v>43266</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K12" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:12" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B13" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C13" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="12">
+        <v>7580</v>
+      </c>
+      <c r="G13" s="12">
+        <v>44446</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K13" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B14" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C14" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="12">
+        <v>42261</v>
+      </c>
+      <c r="G14" s="12">
+        <v>44405</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K14" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B15" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C15" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="12">
+        <v>38056</v>
+      </c>
+      <c r="G15" s="12">
+        <v>40443</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K15" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" s="4" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B16" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C16" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="12">
+        <v>32142</v>
+      </c>
+      <c r="G16" s="12">
+        <v>44452</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K16" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B17" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C17" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="12">
+        <v>42494</v>
+      </c>
+      <c r="G17" s="12">
+        <v>44405</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K17" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B18" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C18" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="12">
+        <v>43787</v>
+      </c>
+      <c r="G18" s="12">
+        <v>43787</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K18" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B19" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C19" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" s="12">
+        <v>41484</v>
+      </c>
+      <c r="G19" s="12">
+        <v>44452</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K19" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="1:12" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B20" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C20" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="12">
+        <v>42331</v>
+      </c>
+      <c r="G20" s="12">
+        <v>42331</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K20" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B21" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C21" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="12">
+        <v>43192</v>
+      </c>
+      <c r="G21" s="12">
+        <v>43192</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K21" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B22" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C22" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="E22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="6">
         <v>39482</v>
       </c>
-      <c r="G8" s="8">
-        <v>39469</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="4">
-        <v>44753</v>
-      </c>
-      <c r="K8" s="4">
-        <v>44753</v>
-      </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-    </row>
-    <row r="9" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>2022</v>
-      </c>
-      <c r="B9" s="4">
-        <v>44652</v>
-      </c>
-      <c r="C9" s="4">
-        <v>44742</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="G22" s="6">
+        <v>39482</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J22" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K22" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B23" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C23" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="E23" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="6">
         <v>39685</v>
       </c>
-      <c r="G9" s="8">
-        <v>39622</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="4">
-        <v>44753</v>
-      </c>
-      <c r="K9" s="4">
-        <v>44753</v>
-      </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-    </row>
-    <row r="10" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>2022</v>
-      </c>
-      <c r="B10" s="4">
-        <v>44652</v>
-      </c>
-      <c r="C10" s="4">
-        <v>44742</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="G23" s="6">
+        <v>39685</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K23" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B24" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C24" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="16">
+        <v>43061</v>
+      </c>
+      <c r="G24" s="16">
+        <v>43061</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K24" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B25" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C25" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="16">
+        <v>42868</v>
+      </c>
+      <c r="G25" s="16">
+        <v>42868</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J25" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K25" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B26" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C26" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="16">
+        <v>40805</v>
+      </c>
+      <c r="G26" s="16">
+        <v>40805</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K26" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B27" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C27" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="16">
+        <v>44440</v>
+      </c>
+      <c r="G27" s="16">
+        <v>44440</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J27" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K27" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B28" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C28" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="16">
+        <v>44448</v>
+      </c>
+      <c r="G28" s="16">
+        <v>44448</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J28" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K28" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B29" s="16">
+        <v>44743</v>
+      </c>
+      <c r="C29" s="16">
+        <v>44834</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" s="16">
         <v>44539</v>
       </c>
-      <c r="G10" s="8">
-        <v>44561</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="4">
-        <v>44753</v>
-      </c>
-      <c r="K10" s="4">
-        <v>44753</v>
-      </c>
-      <c r="L10" s="2"/>
+      <c r="G29" s="16">
+        <v>44539</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J29" s="16">
+        <v>44844</v>
+      </c>
+      <c r="K29" s="16">
+        <v>44844</v>
+      </c>
+      <c r="L29" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="A6:L6"/>
-    <mergeCell ref="M9:Q9"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:I2"/>
@@ -968,12 +1819,36 @@
     <mergeCell ref="G3:I3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D11:D107">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D24:D26 D28:D91">
       <formula1>Hidden_13</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H16" r:id="rId1"/>
+    <hyperlink ref="H8" r:id="rId2"/>
+    <hyperlink ref="H9" r:id="rId3"/>
+    <hyperlink ref="H10" r:id="rId4"/>
+    <hyperlink ref="H11" r:id="rId5"/>
+    <hyperlink ref="H12" r:id="rId6"/>
+    <hyperlink ref="H13" r:id="rId7"/>
+    <hyperlink ref="H14" r:id="rId8"/>
+    <hyperlink ref="H15" r:id="rId9"/>
+    <hyperlink ref="H17" r:id="rId10"/>
+    <hyperlink ref="H18" r:id="rId11"/>
+    <hyperlink ref="H19" r:id="rId12"/>
+    <hyperlink ref="H20" r:id="rId13"/>
+    <hyperlink ref="H21" r:id="rId14"/>
+    <hyperlink ref="H22" r:id="rId15"/>
+    <hyperlink ref="H23" r:id="rId16"/>
+    <hyperlink ref="H24" r:id="rId17"/>
+    <hyperlink ref="H25" r:id="rId18"/>
+    <hyperlink ref="H26" r:id="rId19"/>
+    <hyperlink ref="H27" r:id="rId20"/>
+    <hyperlink ref="H28" r:id="rId21"/>
+    <hyperlink ref="H29" r:id="rId22"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -981,7 +1856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
se crea punto 42
</commit_message>
<xml_diff>
--- a/xlsx/a69_f01UPPachuca.xlsx
+++ b/xlsx/a69_f01UPPachuca.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\2023\SIPOT\2DO TRIMESTRE 2023\Pagina Oficial 2do Trimestre 2023\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\Transparencia UPP\SIPOT\Pagina Oficial 2do tri 23 Vo. Bo Final\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{344D90BA-F384-4A7F-AA32-A250F0597C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FA7D800-ABC0-4271-9038-332061A009B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Formatos" sheetId="1" r:id="rId1"/>
@@ -798,9 +798,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -838,9 +838,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -873,26 +873,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -925,26 +908,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1126,7 +1092,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" style="2" customWidth="1"/>

</xml_diff>